<commit_message>
committing new changes to nodes and variables
</commit_message>
<xml_diff>
--- a/gdcdictionary/xlsx/nodes_schema_impowr.xlsx
+++ b/gdcdictionary/xlsx/nodes_schema_impowr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vithal\Documents\GitHub\dcfdictionary\gdcdictionary\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46938DD9-21C3-469E-9851-71107254CC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3ABEA0-971A-4833-BFE3-7E678EDA5284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="630" windowWidth="10815" windowHeight="13785" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="1605" windowWidth="20745" windowHeight="13785" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes_impowr" sheetId="1" r:id="rId1"/>
@@ -14488,9 +14488,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K958"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A458" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A473" sqref="A473:XFD476"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A619" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20671,10 +20671,10 @@
         <v>281</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="D438" s="4" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="E438" s="3" t="s">
         <v>174</v>
@@ -20685,192 +20685,192 @@
         <v>281</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D439" s="4" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="E439" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="440" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>281</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1112</v>
+        <v>1117</v>
       </c>
       <c r="D440" s="4" t="s">
-        <v>1181</v>
+        <v>1242</v>
       </c>
       <c r="E440" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="441" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>281</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1113</v>
+        <v>1122</v>
       </c>
       <c r="D441" s="4" t="s">
-        <v>1182</v>
+        <v>1190</v>
       </c>
       <c r="E441" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="442" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>281</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1114</v>
+        <v>1121</v>
       </c>
       <c r="D442" s="4" t="s">
-        <v>1183</v>
+        <v>1189</v>
       </c>
       <c r="E442" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="443" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>281</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1115</v>
+        <v>1118</v>
       </c>
       <c r="D443" s="4" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="E443" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="444" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>281</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1116</v>
+        <v>1119</v>
       </c>
       <c r="D444" s="4" t="s">
-        <v>1185</v>
+        <v>1187</v>
       </c>
       <c r="E444" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="445" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>281</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1117</v>
+        <v>1120</v>
       </c>
       <c r="D445" s="4" t="s">
-        <v>1242</v>
+        <v>1188</v>
       </c>
       <c r="E445" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="446" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>281</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1118</v>
+        <v>1126</v>
       </c>
       <c r="D446" s="4" t="s">
-        <v>1186</v>
+        <v>1194</v>
       </c>
       <c r="E446" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="447" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>281</v>
       </c>
       <c r="B447" s="3" t="s">
-        <v>1119</v>
+        <v>1125</v>
       </c>
       <c r="D447" s="4" t="s">
-        <v>1187</v>
+        <v>1193</v>
       </c>
       <c r="E447" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="448" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>281</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1120</v>
+        <v>1128</v>
       </c>
       <c r="D448" s="4" t="s">
-        <v>1188</v>
+        <v>1196</v>
       </c>
       <c r="E448" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="449" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>281</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="D449" s="4" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="E449" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="450" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>281</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1122</v>
+        <v>1127</v>
       </c>
       <c r="D450" s="4" t="s">
-        <v>1190</v>
+        <v>1195</v>
       </c>
       <c r="E450" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="451" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>281</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="D451" s="4" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="E451" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="452" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>281</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1124</v>
+        <v>1114</v>
       </c>
       <c r="D452" s="4" t="s">
-        <v>1192</v>
+        <v>1183</v>
       </c>
       <c r="E452" s="3" t="s">
         <v>174</v>
@@ -20881,13 +20881,13 @@
         <v>281</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1125</v>
+        <v>1113</v>
       </c>
       <c r="D453" s="4" t="s">
-        <v>1193</v>
+        <v>1182</v>
       </c>
       <c r="E453" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="454" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -20895,13 +20895,13 @@
         <v>281</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="D454" s="4" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="E454" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="455" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -20909,10 +20909,10 @@
         <v>281</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1127</v>
+        <v>1112</v>
       </c>
       <c r="D455" s="4" t="s">
-        <v>1195</v>
+        <v>1181</v>
       </c>
       <c r="E455" s="3" t="s">
         <v>174</v>
@@ -20923,10 +20923,10 @@
         <v>281</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1128</v>
+        <v>1116</v>
       </c>
       <c r="D456" s="4" t="s">
-        <v>1196</v>
+        <v>1185</v>
       </c>
       <c r="E456" s="3" t="s">
         <v>174</v>
@@ -20946,7 +20946,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="458" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>346</v>
       </c>
@@ -20960,7 +20960,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>346</v>
       </c>
@@ -20974,7 +20974,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>346</v>
       </c>
@@ -20988,7 +20988,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>346</v>
       </c>
@@ -21002,7 +21002,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="462" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>346</v>
       </c>
@@ -21016,7 +21016,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>346</v>
       </c>
@@ -21030,7 +21030,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>346</v>
       </c>
@@ -21044,7 +21044,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>346</v>
       </c>
@@ -21058,7 +21058,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="466" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>346</v>
       </c>
@@ -21072,7 +21072,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>346</v>
       </c>
@@ -21086,7 +21086,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>346</v>
       </c>
@@ -21100,7 +21100,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>346</v>
       </c>
@@ -21114,7 +21114,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>346</v>
       </c>
@@ -21128,7 +21128,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>346</v>
       </c>
@@ -21142,7 +21142,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>346</v>
       </c>
@@ -23200,7 +23200,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="619" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
         <v>298</v>
       </c>
@@ -23214,7 +23214,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="620" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
         <v>298</v>
       </c>
@@ -23228,7 +23228,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="621" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
         <v>298</v>
       </c>
@@ -23242,7 +23242,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="622" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
         <v>298</v>
       </c>
@@ -23256,7 +23256,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="623" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
         <v>298</v>
       </c>
@@ -23270,7 +23270,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="624" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
         <v>298</v>
       </c>
@@ -27964,9 +27964,12 @@
   <autoFilter ref="A1:K958" xr:uid="{00000000-0001-0000-0100-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="pb_aim_iam_fim"/>
+        <filter val="pb_pain_catastrophizing"/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A437:K457">
+      <sortCondition ref="B1:B958"/>
+    </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27978,7 +27981,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E2044"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1101" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A1116" sqref="A1116:XFD1130"/>
     </sheetView>
@@ -40332,7 +40335,7 @@
       </c>
       <c r="D1055" s="3"/>
     </row>
-    <row r="1056" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1056" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1056" t="s">
         <v>346</v>
       </c>
@@ -40346,7 +40349,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1057" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1057" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1057" t="s">
         <v>346</v>
       </c>
@@ -40358,7 +40361,7 @@
       </c>
       <c r="D1057" s="3"/>
     </row>
-    <row r="1058" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1058" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1058" t="s">
         <v>346</v>
       </c>
@@ -40370,7 +40373,7 @@
       </c>
       <c r="D1058" s="3"/>
     </row>
-    <row r="1059" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1059" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1059" t="s">
         <v>346</v>
       </c>
@@ -40382,7 +40385,7 @@
       </c>
       <c r="D1059" s="3"/>
     </row>
-    <row r="1060" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1060" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1060" t="s">
         <v>346</v>
       </c>
@@ -40394,7 +40397,7 @@
       </c>
       <c r="D1060" s="3"/>
     </row>
-    <row r="1061" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1061" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1061" t="s">
         <v>346</v>
       </c>
@@ -40408,7 +40411,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1062" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1062" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1062" t="s">
         <v>346</v>
       </c>
@@ -40420,7 +40423,7 @@
       </c>
       <c r="D1062" s="3"/>
     </row>
-    <row r="1063" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1063" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1063" t="s">
         <v>346</v>
       </c>
@@ -40432,7 +40435,7 @@
       </c>
       <c r="D1063" s="3"/>
     </row>
-    <row r="1064" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1064" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1064" t="s">
         <v>346</v>
       </c>
@@ -40444,7 +40447,7 @@
       </c>
       <c r="D1064" s="3"/>
     </row>
-    <row r="1065" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1065" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1065" t="s">
         <v>346</v>
       </c>
@@ -40456,7 +40459,7 @@
       </c>
       <c r="D1065" s="3"/>
     </row>
-    <row r="1066" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1066" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1066" t="s">
         <v>346</v>
       </c>
@@ -40470,7 +40473,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1067" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1067" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1067" t="s">
         <v>346</v>
       </c>
@@ -40482,7 +40485,7 @@
       </c>
       <c r="D1067" s="3"/>
     </row>
-    <row r="1068" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1068" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1068" t="s">
         <v>346</v>
       </c>
@@ -40494,7 +40497,7 @@
       </c>
       <c r="D1068" s="3"/>
     </row>
-    <row r="1069" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1069" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1069" t="s">
         <v>346</v>
       </c>
@@ -40506,7 +40509,7 @@
       </c>
       <c r="D1069" s="3"/>
     </row>
-    <row r="1070" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1070" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1070" t="s">
         <v>346</v>
       </c>
@@ -40518,7 +40521,7 @@
       </c>
       <c r="D1070" s="3"/>
     </row>
-    <row r="1071" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1071" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1071" t="s">
         <v>346</v>
       </c>
@@ -40532,7 +40535,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1072" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1072" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1072" t="s">
         <v>346</v>
       </c>
@@ -40544,7 +40547,7 @@
       </c>
       <c r="D1072" s="3"/>
     </row>
-    <row r="1073" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1073" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1073" t="s">
         <v>346</v>
       </c>
@@ -40556,7 +40559,7 @@
       </c>
       <c r="D1073" s="3"/>
     </row>
-    <row r="1074" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1074" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1074" t="s">
         <v>346</v>
       </c>
@@ -40568,7 +40571,7 @@
       </c>
       <c r="D1074" s="3"/>
     </row>
-    <row r="1075" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1075" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1075" t="s">
         <v>346</v>
       </c>
@@ -40580,7 +40583,7 @@
       </c>
       <c r="D1075" s="3"/>
     </row>
-    <row r="1076" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1076" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1076" t="s">
         <v>346</v>
       </c>
@@ -40594,7 +40597,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1077" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1077" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1077" t="s">
         <v>346</v>
       </c>
@@ -40606,7 +40609,7 @@
       </c>
       <c r="D1077" s="3"/>
     </row>
-    <row r="1078" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1078" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1078" t="s">
         <v>346</v>
       </c>
@@ -40618,7 +40621,7 @@
       </c>
       <c r="D1078" s="3"/>
     </row>
-    <row r="1079" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1079" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1079" t="s">
         <v>346</v>
       </c>
@@ -40630,7 +40633,7 @@
       </c>
       <c r="D1079" s="3"/>
     </row>
-    <row r="1080" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1080" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1080" t="s">
         <v>346</v>
       </c>
@@ -40642,7 +40645,7 @@
       </c>
       <c r="D1080" s="3"/>
     </row>
-    <row r="1081" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1081" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1081" t="s">
         <v>346</v>
       </c>
@@ -40656,7 +40659,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1082" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1082" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1082" t="s">
         <v>346</v>
       </c>
@@ -40668,7 +40671,7 @@
       </c>
       <c r="D1082" s="3"/>
     </row>
-    <row r="1083" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1083" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1083" t="s">
         <v>346</v>
       </c>
@@ -40680,7 +40683,7 @@
       </c>
       <c r="D1083" s="3"/>
     </row>
-    <row r="1084" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1084" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1084" t="s">
         <v>346</v>
       </c>
@@ -40692,7 +40695,7 @@
       </c>
       <c r="D1084" s="3"/>
     </row>
-    <row r="1085" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1085" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1085" t="s">
         <v>346</v>
       </c>
@@ -40704,7 +40707,7 @@
       </c>
       <c r="D1085" s="3"/>
     </row>
-    <row r="1086" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1086" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1086" t="s">
         <v>346</v>
       </c>
@@ -40718,7 +40721,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1087" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1087" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1087" t="s">
         <v>346</v>
       </c>
@@ -40730,7 +40733,7 @@
       </c>
       <c r="D1087" s="3"/>
     </row>
-    <row r="1088" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1088" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1088" t="s">
         <v>346</v>
       </c>
@@ -40742,7 +40745,7 @@
       </c>
       <c r="D1088" s="3"/>
     </row>
-    <row r="1089" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1089" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1089" t="s">
         <v>346</v>
       </c>
@@ -40754,7 +40757,7 @@
       </c>
       <c r="D1089" s="3"/>
     </row>
-    <row r="1090" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1090" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1090" t="s">
         <v>346</v>
       </c>
@@ -40766,7 +40769,7 @@
       </c>
       <c r="D1090" s="3"/>
     </row>
-    <row r="1091" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1091" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1091" t="s">
         <v>346</v>
       </c>
@@ -40780,7 +40783,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1092" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1092" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1092" t="s">
         <v>346</v>
       </c>
@@ -40792,7 +40795,7 @@
       </c>
       <c r="D1092" s="3"/>
     </row>
-    <row r="1093" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1093" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1093" t="s">
         <v>346</v>
       </c>
@@ -40804,7 +40807,7 @@
       </c>
       <c r="D1093" s="3"/>
     </row>
-    <row r="1094" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1094" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1094" t="s">
         <v>346</v>
       </c>
@@ -40816,7 +40819,7 @@
       </c>
       <c r="D1094" s="3"/>
     </row>
-    <row r="1095" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1095" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1095" t="s">
         <v>346</v>
       </c>
@@ -40828,7 +40831,7 @@
       </c>
       <c r="D1095" s="3"/>
     </row>
-    <row r="1096" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1096" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1096" t="s">
         <v>346</v>
       </c>
@@ -40842,7 +40845,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1097" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1097" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1097" t="s">
         <v>346</v>
       </c>
@@ -40854,7 +40857,7 @@
       </c>
       <c r="D1097" s="3"/>
     </row>
-    <row r="1098" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1098" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1098" t="s">
         <v>346</v>
       </c>
@@ -40866,7 +40869,7 @@
       </c>
       <c r="D1098" s="3"/>
     </row>
-    <row r="1099" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1099" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1099" t="s">
         <v>346</v>
       </c>
@@ -40878,7 +40881,7 @@
       </c>
       <c r="D1099" s="3"/>
     </row>
-    <row r="1100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1100" t="s">
         <v>346</v>
       </c>
@@ -40890,7 +40893,7 @@
       </c>
       <c r="D1100" s="3"/>
     </row>
-    <row r="1101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1101" t="s">
         <v>346</v>
       </c>
@@ -40904,7 +40907,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1102" t="s">
         <v>346</v>
       </c>
@@ -40916,7 +40919,7 @@
       </c>
       <c r="D1102" s="3"/>
     </row>
-    <row r="1103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1103" t="s">
         <v>346</v>
       </c>
@@ -40928,7 +40931,7 @@
       </c>
       <c r="D1103" s="3"/>
     </row>
-    <row r="1104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1104" t="s">
         <v>346</v>
       </c>
@@ -40940,7 +40943,7 @@
       </c>
       <c r="D1104" s="3"/>
     </row>
-    <row r="1105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1105" t="s">
         <v>346</v>
       </c>
@@ -40952,7 +40955,7 @@
       </c>
       <c r="D1105" s="3"/>
     </row>
-    <row r="1106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1106" t="s">
         <v>346</v>
       </c>
@@ -40966,7 +40969,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1107" t="s">
         <v>346</v>
       </c>
@@ -40978,7 +40981,7 @@
       </c>
       <c r="D1107" s="3"/>
     </row>
-    <row r="1108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1108" t="s">
         <v>346</v>
       </c>
@@ -40990,7 +40993,7 @@
       </c>
       <c r="D1108" s="3"/>
     </row>
-    <row r="1109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1109" t="s">
         <v>346</v>
       </c>
@@ -41002,7 +41005,7 @@
       </c>
       <c r="D1109" s="3"/>
     </row>
-    <row r="1110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1110" t="s">
         <v>346</v>
       </c>
@@ -41014,7 +41017,7 @@
       </c>
       <c r="D1110" s="3"/>
     </row>
-    <row r="1111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1111" t="s">
         <v>346</v>
       </c>
@@ -41028,7 +41031,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="1112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1112" t="s">
         <v>346</v>
       </c>
@@ -41040,7 +41043,7 @@
       </c>
       <c r="D1112" s="3"/>
     </row>
-    <row r="1113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1113" t="s">
         <v>346</v>
       </c>
@@ -41052,7 +41055,7 @@
       </c>
       <c r="D1113" s="3"/>
     </row>
-    <row r="1114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1114" t="s">
         <v>346</v>
       </c>
@@ -41064,7 +41067,7 @@
       </c>
       <c r="D1114" s="3"/>
     </row>
-    <row r="1115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1115" t="s">
         <v>346</v>
       </c>
@@ -48168,7 +48171,7 @@
       </c>
       <c r="D1692" s="3"/>
     </row>
-    <row r="1693" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1693" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1693" t="s">
         <v>317</v>
       </c>
@@ -48182,7 +48185,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="1694" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1694" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1694" t="s">
         <v>317</v>
       </c>
@@ -48194,7 +48197,7 @@
       </c>
       <c r="D1694" s="3"/>
     </row>
-    <row r="1695" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1695" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1695" t="s">
         <v>317</v>
       </c>
@@ -48206,7 +48209,7 @@
       </c>
       <c r="D1695" s="3"/>
     </row>
-    <row r="1696" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1696" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1696" t="s">
         <v>317</v>
       </c>
@@ -48218,7 +48221,7 @@
       </c>
       <c r="D1696" s="3"/>
     </row>
-    <row r="1697" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1697" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1697" t="s">
         <v>317</v>
       </c>
@@ -48230,7 +48233,7 @@
       </c>
       <c r="D1697" s="3"/>
     </row>
-    <row r="1698" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1698" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1698" t="s">
         <v>317</v>
       </c>
@@ -48242,7 +48245,7 @@
       </c>
       <c r="D1698" s="3"/>
     </row>
-    <row r="1699" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1699" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1699" t="s">
         <v>317</v>
       </c>
@@ -48254,7 +48257,7 @@
       </c>
       <c r="D1699" s="3"/>
     </row>
-    <row r="1700" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1700" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1700" t="s">
         <v>317</v>
       </c>
@@ -48268,7 +48271,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="1701" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1701" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1701" t="s">
         <v>317</v>
       </c>
@@ -48280,7 +48283,7 @@
       </c>
       <c r="D1701" s="3"/>
     </row>
-    <row r="1702" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1702" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1702" t="s">
         <v>317</v>
       </c>
@@ -48292,7 +48295,7 @@
       </c>
       <c r="D1702" s="3"/>
     </row>
-    <row r="1703" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1703" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1703" t="s">
         <v>317</v>
       </c>
@@ -48304,7 +48307,7 @@
       </c>
       <c r="D1703" s="3"/>
     </row>
-    <row r="1704" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1704" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1704" t="s">
         <v>317</v>
       </c>
@@ -48316,7 +48319,7 @@
       </c>
       <c r="D1704" s="3"/>
     </row>
-    <row r="1705" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1705" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1705" t="s">
         <v>317</v>
       </c>
@@ -48328,7 +48331,7 @@
       </c>
       <c r="D1705" s="3"/>
     </row>
-    <row r="1706" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1706" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1706" t="s">
         <v>317</v>
       </c>
@@ -48340,7 +48343,7 @@
       </c>
       <c r="D1706" s="3"/>
     </row>
-    <row r="1707" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1707" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1707" t="s">
         <v>317</v>
       </c>
@@ -48354,7 +48357,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="1708" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1708" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1708" t="s">
         <v>317</v>
       </c>
@@ -48366,7 +48369,7 @@
       </c>
       <c r="D1708" s="3"/>
     </row>
-    <row r="1709" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1709" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1709" t="s">
         <v>317</v>
       </c>
@@ -48378,7 +48381,7 @@
       </c>
       <c r="D1709" s="3"/>
     </row>
-    <row r="1710" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1710" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1710" t="s">
         <v>317</v>
       </c>
@@ -48390,7 +48393,7 @@
       </c>
       <c r="D1710" s="3"/>
     </row>
-    <row r="1711" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1711" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1711" t="s">
         <v>317</v>
       </c>
@@ -48402,7 +48405,7 @@
       </c>
       <c r="D1711" s="3"/>
     </row>
-    <row r="1712" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1712" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1712" t="s">
         <v>317</v>
       </c>
@@ -48414,7 +48417,7 @@
       </c>
       <c r="D1712" s="3"/>
     </row>
-    <row r="1713" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1713" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1713" t="s">
         <v>317</v>
       </c>
@@ -52541,7 +52544,7 @@
   <autoFilter ref="A1:E2044" xr:uid="{00000000-0001-0000-0200-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="pb_aim_iam_fim"/>
+        <filter val="pb_audit_c"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>